<commit_message>
[DOM-304] add structured acceptance tests document
</commit_message>
<xml_diff>
--- a/documentation/acceptance/Tracing.xlsx
+++ b/documentation/acceptance/Tracing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\3year_part2\TP\TP-9.1\documentation\acceptance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE1B8CBF-8A36-4F43-A490-DB92DA6DCF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A33B7C-A86E-43FC-AA08-1BA60692F2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E7EDFB0B-D52E-4F7D-A88B-AA155C5CCBE2}"/>
   </bookViews>
@@ -25,12 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Требование в ТЗ</t>
   </si>
   <si>
     <t>Сценарии в ПМИ</t>
+  </si>
+  <si>
+    <t>not_auth_1</t>
+  </si>
+  <si>
+    <t>ТС-А1, ТС-А2, ТС-А3, ТС-А4</t>
+  </si>
+  <si>
+    <t>not_auth_2</t>
+  </si>
+  <si>
+    <t>ТС-Р1, ТС-Р2, ТС-Р3</t>
+  </si>
+  <si>
+    <t>not_auth_3</t>
+  </si>
+  <si>
+    <t>ТС-ОБ1, ТС-ОБ2</t>
+  </si>
+  <si>
+    <t>not_auth_4</t>
+  </si>
+  <si>
+    <t>ТС-ПР1, ТС-ПР2, ТС-ПР3</t>
+  </si>
+  <si>
+    <t>not_auth_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5.1 ТС-ФИ1 </t>
   </si>
 </sst>
 </file>
@@ -383,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FF33F1-9503-44AA-97D2-2E99869C08DD}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,6 +433,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[DOM-304] add all acceptance scenarios skeleton and there tracing to ts
</commit_message>
<xml_diff>
--- a/documentation/acceptance/Tracing.xlsx
+++ b/documentation/acceptance/Tracing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\3year_part2\TP\TP-9.1\documentation\acceptance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A33B7C-A86E-43FC-AA08-1BA60692F2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEECBE7-9BD4-4CA6-BC8A-95AC3D3D8904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E7EDFB0B-D52E-4F7D-A88B-AA155C5CCBE2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Требование в ТЗ</t>
   </si>
@@ -48,9 +48,6 @@
     <t>not_auth_3</t>
   </si>
   <si>
-    <t>ТС-ОБ1, ТС-ОБ2</t>
-  </si>
-  <si>
     <t>not_auth_4</t>
   </si>
   <si>
@@ -60,17 +57,170 @@
     <t>not_auth_5</t>
   </si>
   <si>
-    <t xml:space="preserve">6.5.1 ТС-ФИ1 </t>
+    <t>not_auth_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТС-ФИ1 </t>
+  </si>
+  <si>
+    <t>ТС-СОР1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not_auth_7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТС- КА1 </t>
+  </si>
+  <si>
+    <t>auth_1</t>
+  </si>
+  <si>
+    <t>ТС-ПРОФ1, ТС-ПРОФ2, ТС-ПРОФ3</t>
+  </si>
+  <si>
+    <t>auth_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТС- ОБ-ПР1, ТС- ОБ-ПР2, ТС- ОБ-ПР3, ТС- ОБ-ПР4 </t>
+  </si>
+  <si>
+    <t>auth_3</t>
+  </si>
+  <si>
+    <t>auth_4</t>
+  </si>
+  <si>
+    <t>ТС-ПР1</t>
+  </si>
+  <si>
+    <t>auth_5</t>
+  </si>
+  <si>
+    <t>auth_6</t>
+  </si>
+  <si>
+    <t>ТС-ПУБ1, ТС-ПУБ2, ТС-ПУБ3</t>
+  </si>
+  <si>
+    <t>ТС-РЕД1, ТС-РЕД2, ТС-РЕД3</t>
+  </si>
+  <si>
+    <t>auth_7</t>
+  </si>
+  <si>
+    <t>ТС-УД1, ТС-УД2</t>
+  </si>
+  <si>
+    <t>auth_8</t>
+  </si>
+  <si>
+    <t>ТС-ОБ3, ТС-ОБ4</t>
+  </si>
+  <si>
+    <t>ТС-ОБ1, ТС-ОБ2, ТС-ОБ5</t>
+  </si>
+  <si>
+    <t>ТС-ОБ-СВ1, ТС-ОБ-СВ2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auth_9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">auth_10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТС-ОТКЛ1 </t>
+  </si>
+  <si>
+    <t>auth_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТС-ОТКЛ-П1 </t>
+  </si>
+  <si>
+    <t>auth_12</t>
+  </si>
+  <si>
+    <t>auth_13</t>
+  </si>
+  <si>
+    <t>ТС-ОТКЛ-П2</t>
+  </si>
+  <si>
+    <t>ТС-НАСТР1, ТС-НАСТР2, ТС-НАСТР3, ТС-НАСТР4</t>
+  </si>
+  <si>
+    <t>auth_14</t>
+  </si>
+  <si>
+    <t>ТС-ИЗБР1, ТС-ИЗБР2, ТС-ИЗБР3, ТС-ИЗБР4</t>
+  </si>
+  <si>
+    <t>auth_15</t>
+  </si>
+  <si>
+    <t>ТС-ИЗБР-СП1, ТС-ИЗБР-СП2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auth_16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТС-ОТКЛ-СП1, ТС-ОТКЛ-СП2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">auth_17 </t>
+  </si>
+  <si>
+    <t>ТС-ОТКЛ-АКТ1, ТС-ОТКЛ-АКТ2, ТС-ОТКЛ-АКТ3, ТС-ОТКЛ-АКТ4, ТС-ОТКЛ-АКТ5, ТС-ОТКЛ-АКТ6</t>
+  </si>
+  <si>
+    <t>admin_1</t>
+  </si>
+  <si>
+    <t>admin_2</t>
+  </si>
+  <si>
+    <t>admin_3</t>
+  </si>
+  <si>
+    <t>admin_4</t>
+  </si>
+  <si>
+    <t>admin_5</t>
+  </si>
+  <si>
+    <t>ТС-А-ОБ-БЛ1, ТС-А-ОБ-БЛ2, ТС-А-ОБ-БЛ3,
+ТС-А-ОБ-БЛ4</t>
+  </si>
+  <si>
+    <t>ТС-А-ОБ-УД1, ТС-А-ОБ-УД2</t>
+  </si>
+  <si>
+    <t>ТС-А-ПОЛ-БЛ1, ТС-А-ПОЛ-БЛ2, ТС-А-ПОЛ-БЛ3,
+ТС-А-ПОЛ-БЛ4</t>
+  </si>
+  <si>
+    <t>ТС-А-ПОЛ-УД1, ТС-А-ПОЛ-УД2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТС-А-ФИ1 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -97,8 +247,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -413,16 +566,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FF33F1-9503-44AA-97D2-2E99869C08DD}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="38.109375" customWidth="1"/>
+    <col min="2" max="2" width="42.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -454,26 +607,219 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[DOM-306] Finish acceptance csenarios
</commit_message>
<xml_diff>
--- a/documentation/acceptance/Tracing.xlsx
+++ b/documentation/acceptance/Tracing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\3year_part2\TP\TP-9.1\documentation\acceptance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEECBE7-9BD4-4CA6-BC8A-95AC3D3D8904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300A5265-6F86-4E53-BC7A-6BB056042DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E7EDFB0B-D52E-4F7D-A88B-AA155C5CCBE2}"/>
   </bookViews>
@@ -147,9 +147,6 @@
     <t>ТС-ОТКЛ-П2</t>
   </si>
   <si>
-    <t>ТС-НАСТР1, ТС-НАСТР2, ТС-НАСТР3, ТС-НАСТР4</t>
-  </si>
-  <si>
     <t>auth_14</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t xml:space="preserve">ТС-А-ФИ1 </t>
+  </si>
+  <si>
+    <t>ТС-НАСТР1, ТС-НАСТР2</t>
   </si>
 </sst>
 </file>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FF33F1-9503-44AA-97D2-2E99869C08DD}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,79 +743,79 @@
         <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
         <v>45</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[DOM-306] Add AI test to acceptance
</commit_message>
<xml_diff>
--- a/documentation/acceptance/Tracing.xlsx
+++ b/documentation/acceptance/Tracing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\3year_part2\TP\TP-9.1\documentation\acceptance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300A5265-6F86-4E53-BC7A-6BB056042DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7DD3B0-C935-462A-BC1F-09DFB403CA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E7EDFB0B-D52E-4F7D-A88B-AA155C5CCBE2}"/>
   </bookViews>
@@ -99,12 +99,6 @@
     <t>auth_6</t>
   </si>
   <si>
-    <t>ТС-ПУБ1, ТС-ПУБ2, ТС-ПУБ3</t>
-  </si>
-  <si>
-    <t>ТС-РЕД1, ТС-РЕД2, ТС-РЕД3</t>
-  </si>
-  <si>
     <t>auth_7</t>
   </si>
   <si>
@@ -204,6 +198,12 @@
   </si>
   <si>
     <t>ТС-НАСТР1, ТС-НАСТР2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТС-ПУБ1, ТС-ПУБ2, ТС-ПУБ3, ТС-АВТО-1 </t>
+  </si>
+  <si>
+    <t>ТС-РЕД1, ТС-РЕД2, ТС-РЕД3,  ТС-АВТО-12</t>
   </si>
 </sst>
 </file>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FF33F1-9503-44AA-97D2-2E99869C08DD}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +607,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -663,7 +663,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -679,7 +679,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -687,135 +687,135 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
         <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[DOM-306] Fix acceptance style
</commit_message>
<xml_diff>
--- a/documentation/acceptance/Tracing.xlsx
+++ b/documentation/acceptance/Tracing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\3year_part2\TP\TP-9.1\documentation\acceptance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7DD3B0-C935-462A-BC1F-09DFB403CA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2744D1FB-1CB0-48E1-B4E4-246AADA7073F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E7EDFB0B-D52E-4F7D-A88B-AA155C5CCBE2}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>auth_2</t>
   </si>
   <si>
-    <t xml:space="preserve">ТС- ОБ-ПР1, ТС- ОБ-ПР2, ТС- ОБ-ПР3, ТС- ОБ-ПР4 </t>
-  </si>
-  <si>
     <t>auth_3</t>
   </si>
   <si>
@@ -123,22 +120,13 @@
     <t xml:space="preserve">auth_10 </t>
   </si>
   <si>
-    <t xml:space="preserve">ТС-ОТКЛ1 </t>
-  </si>
-  <si>
     <t>auth_11</t>
   </si>
   <si>
-    <t xml:space="preserve">ТС-ОТКЛ-П1 </t>
-  </si>
-  <si>
     <t>auth_12</t>
   </si>
   <si>
     <t>auth_13</t>
-  </si>
-  <si>
-    <t>ТС-ОТКЛ-П2</t>
   </si>
   <si>
     <t>auth_14</t>
@@ -204,6 +192,18 @@
   </si>
   <si>
     <t>ТС-РЕД1, ТС-РЕД2, ТС-РЕД3,  ТС-АВТО-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТС- ОБ-ПР1, ТС- ОБ-ПР2, ТС- ОБ-ПР3 </t>
+  </si>
+  <si>
+    <t>ТС-ДАТ-В1</t>
+  </si>
+  <si>
+    <t>ТС-НАСТР1</t>
+  </si>
+  <si>
+    <t>ТС-НАСТР2</t>
   </si>
 </sst>
 </file>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FF33F1-9503-44AA-97D2-2E99869C08DD}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +607,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -655,167 +655,167 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
         <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>